<commit_message>
Remove testcase from xl
</commit_message>
<xml_diff>
--- a/resources/testdata/reserve_invalid_data.xlsx
+++ b/resources/testdata/reserve_invalid_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravindra\Downloads\ApiFramework\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravindra\PycharmProjects\ApiAutomation\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>PUT</t>
   </si>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>RESPONSE</t>
-  </si>
-  <si>
-    <t>{"action":"reserve","validity_in_minutes":10,"vendor_data":{"$vendor_id":"$device_id"},"rfids":["$rfid_key","456"],"rental_id":1234,"key_validity_start_in_epoch":-1,"key_validity_stop_in_epoch":1550668696}</t>
   </si>
   <si>
     <t>Invalid epoch timestamp for key validity start/stop timestamp</t>
@@ -412,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +477,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -497,32 +494,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed failing case from excel
</commit_message>
<xml_diff>
--- a/resources/testdata/reserve_invalid_data.xlsx
+++ b/resources/testdata/reserve_invalid_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>PUT</t>
   </si>
@@ -76,12 +76,6 @@
   </si>
   <si>
     <t>RESPONSE</t>
-  </si>
-  <si>
-    <t>Invalid epoch timestamp for key validity start/stop timestamp</t>
-  </si>
-  <si>
-    <t>{"action":"reserve","validity_in_minutes":-10,"vendor_data":{"$vendor_id":"$device_id"},"rfids":["$rfid_key","456"],"rental_id":1234,"key_validity_start_in_epoch":1550643333,"key_validity_stop_in_epoch":-1}</t>
   </si>
 </sst>
 </file>
@@ -123,12 +117,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,31 +461,6 @@
       </c>
       <c r="C4" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>